<commit_message>
Update premium table data
</commit_message>
<xml_diff>
--- a/premiumtable.xlsx
+++ b/premiumtable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chakh\OneDrive\桌面\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chakh\OneDrive\桌面\streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76F4647-9D84-4299-899B-EFEEE777929A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B792D51-7063-493B-9C89-108318DCA438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{2B5941AF-E55B-4360-8715-EE7BF2DCC1DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2B5941AF-E55B-4360-8715-EE7BF2DCC1DA}"/>
   </bookViews>
   <sheets>
     <sheet name="female" sheetId="2" r:id="rId1"/>
@@ -1718,8 +1718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AB666C-B717-4DAB-B43C-8A2A713B7A3F}">
   <dimension ref="A1:AZ101"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1895,10 +1895,10 @@
         <v>3841</v>
       </c>
       <c r="C2" s="5">
-        <v>3624</v>
+        <v>3950</v>
       </c>
       <c r="D2" s="5">
-        <v>6289</v>
+        <v>6855</v>
       </c>
       <c r="E2" s="5">
         <v>8703</v>
@@ -2053,10 +2053,10 @@
         <v>3841</v>
       </c>
       <c r="C3" s="7">
-        <v>3624</v>
+        <v>3950</v>
       </c>
       <c r="D3" s="7">
-        <v>6289</v>
+        <v>6855</v>
       </c>
       <c r="E3" s="7">
         <v>8703</v>
@@ -2211,10 +2211,10 @@
         <v>3841</v>
       </c>
       <c r="C4" s="7">
-        <v>3624</v>
+        <v>3950</v>
       </c>
       <c r="D4" s="7">
-        <v>6289</v>
+        <v>6855</v>
       </c>
       <c r="E4" s="7">
         <v>8703</v>
@@ -2369,10 +2369,10 @@
         <v>3841</v>
       </c>
       <c r="C5" s="7">
-        <v>3624</v>
+        <v>3950</v>
       </c>
       <c r="D5" s="7">
-        <v>6289</v>
+        <v>6855</v>
       </c>
       <c r="E5" s="7">
         <v>8703</v>
@@ -2527,10 +2527,10 @@
         <v>4394</v>
       </c>
       <c r="C6" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D6" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E6" s="7">
         <v>8703</v>
@@ -2685,10 +2685,10 @@
         <v>4394</v>
       </c>
       <c r="C7" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D7" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E7" s="7">
         <v>7956</v>
@@ -2843,10 +2843,10 @@
         <v>4394</v>
       </c>
       <c r="C8" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D8" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E8" s="7">
         <v>7956</v>
@@ -3001,10 +3001,10 @@
         <v>4394</v>
       </c>
       <c r="C9" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D9" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E9" s="7">
         <v>7956</v>
@@ -3159,10 +3159,10 @@
         <v>4394</v>
       </c>
       <c r="C10" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D10" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E10" s="7">
         <v>7956</v>
@@ -3317,10 +3317,10 @@
         <v>4394</v>
       </c>
       <c r="C11" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D11" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E11" s="7">
         <v>7956</v>
@@ -3475,10 +3475,10 @@
         <v>4394</v>
       </c>
       <c r="C12" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D12" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E12" s="7">
         <v>7956</v>
@@ -3633,10 +3633,10 @@
         <v>4394</v>
       </c>
       <c r="C13" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D13" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E13" s="7">
         <v>7956</v>
@@ -3791,10 +3791,10 @@
         <v>4394</v>
       </c>
       <c r="C14" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D14" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E14" s="7">
         <v>7956</v>
@@ -3949,10 +3949,10 @@
         <v>4394</v>
       </c>
       <c r="C15" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D15" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E15" s="7">
         <v>7956</v>
@@ -4107,10 +4107,10 @@
         <v>4394</v>
       </c>
       <c r="C16" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D16" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E16" s="7">
         <v>7956</v>
@@ -4265,10 +4265,10 @@
         <v>4394</v>
       </c>
       <c r="C17" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D17" s="7">
-        <v>6148</v>
+        <v>6886</v>
       </c>
       <c r="E17" s="7">
         <v>7956</v>
@@ -4423,10 +4423,10 @@
         <v>4394</v>
       </c>
       <c r="C18" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D18" s="7">
-        <v>6063</v>
+        <v>6791</v>
       </c>
       <c r="E18" s="7">
         <v>7956</v>
@@ -4581,10 +4581,10 @@
         <v>4394</v>
       </c>
       <c r="C19" s="7">
-        <v>4035</v>
+        <v>4519</v>
       </c>
       <c r="D19" s="7">
-        <v>6034</v>
+        <v>6758</v>
       </c>
       <c r="E19" s="7">
         <v>7956</v>
@@ -4739,10 +4739,10 @@
         <v>4420</v>
       </c>
       <c r="C20" s="7">
-        <v>4059</v>
+        <v>4546</v>
       </c>
       <c r="D20" s="7">
-        <v>6008</v>
+        <v>6729</v>
       </c>
       <c r="E20" s="7">
         <v>8177</v>
@@ -4897,10 +4897,10 @@
         <v>4446</v>
       </c>
       <c r="C21" s="7">
-        <v>4083</v>
+        <v>4573</v>
       </c>
       <c r="D21" s="7">
-        <v>6114</v>
+        <v>6848</v>
       </c>
       <c r="E21" s="7">
         <v>8244</v>
@@ -5055,10 +5055,10 @@
         <v>4473</v>
       </c>
       <c r="C22" s="7">
-        <v>4107</v>
+        <v>4600</v>
       </c>
       <c r="D22" s="7">
-        <v>6418</v>
+        <v>7188</v>
       </c>
       <c r="E22" s="7">
         <v>8437</v>
@@ -5213,10 +5213,10 @@
         <v>4500</v>
       </c>
       <c r="C23" s="7">
-        <v>4132</v>
+        <v>4628</v>
       </c>
       <c r="D23" s="7">
-        <v>6722</v>
+        <v>7529</v>
       </c>
       <c r="E23" s="7">
         <v>8697</v>
@@ -5371,10 +5371,10 @@
         <v>4520</v>
       </c>
       <c r="C24" s="7">
-        <v>4151</v>
+        <v>4649</v>
       </c>
       <c r="D24" s="7">
-        <v>6739</v>
+        <v>7548</v>
       </c>
       <c r="E24" s="7">
         <v>8948</v>
@@ -5529,10 +5529,10 @@
         <v>4659</v>
       </c>
       <c r="C25" s="7">
-        <v>4278</v>
+        <v>4791</v>
       </c>
       <c r="D25" s="7">
-        <v>6756</v>
+        <v>7567</v>
       </c>
       <c r="E25" s="7">
         <v>9131</v>
@@ -5687,10 +5687,10 @@
         <v>4855</v>
       </c>
       <c r="C26" s="7">
-        <v>4458</v>
+        <v>4993</v>
       </c>
       <c r="D26" s="7">
-        <v>6959</v>
+        <v>7794</v>
       </c>
       <c r="E26" s="7">
         <v>9267</v>
@@ -5845,10 +5845,10 @@
         <v>5184</v>
       </c>
       <c r="C27" s="7">
-        <v>4760</v>
+        <v>5331</v>
       </c>
       <c r="D27" s="7">
-        <v>7026</v>
+        <v>7869</v>
       </c>
       <c r="E27" s="7">
         <v>9723</v>
@@ -6003,10 +6003,10 @@
         <v>5459</v>
       </c>
       <c r="C28" s="7">
-        <v>5013</v>
+        <v>5615</v>
       </c>
       <c r="D28" s="7">
-        <v>7093</v>
+        <v>7944</v>
       </c>
       <c r="E28" s="7">
         <v>10254</v>
@@ -6161,10 +6161,10 @@
         <v>5751</v>
       </c>
       <c r="C29" s="7">
-        <v>5281</v>
+        <v>5915</v>
       </c>
       <c r="D29" s="7">
-        <v>7653</v>
+        <v>8571</v>
       </c>
       <c r="E29" s="7">
         <v>10778</v>
@@ -6319,10 +6319,10 @@
         <v>6015</v>
       </c>
       <c r="C30" s="7">
-        <v>5523</v>
+        <v>6186</v>
       </c>
       <c r="D30" s="7">
-        <v>8049</v>
+        <v>9015</v>
       </c>
       <c r="E30" s="7">
         <v>11167</v>
@@ -6477,10 +6477,10 @@
         <v>6302</v>
       </c>
       <c r="C31" s="7">
-        <v>5787</v>
+        <v>6481</v>
       </c>
       <c r="D31" s="7">
-        <v>8306</v>
+        <v>9303</v>
       </c>
       <c r="E31" s="7">
         <v>11417</v>
@@ -6635,10 +6635,10 @@
         <v>6464</v>
       </c>
       <c r="C32" s="7">
-        <v>5936</v>
+        <v>6648</v>
       </c>
       <c r="D32" s="7">
-        <v>8562</v>
+        <v>9589</v>
       </c>
       <c r="E32" s="7">
         <v>11587</v>
@@ -6793,10 +6793,10 @@
         <v>6655</v>
       </c>
       <c r="C33" s="7">
-        <v>6111</v>
+        <v>6844</v>
       </c>
       <c r="D33" s="7">
-        <v>8816</v>
+        <v>9874</v>
       </c>
       <c r="E33" s="7">
         <v>11851</v>
@@ -6951,10 +6951,10 @@
         <v>6868</v>
       </c>
       <c r="C34" s="7">
-        <v>6307</v>
+        <v>7064</v>
       </c>
       <c r="D34" s="7">
-        <v>9072</v>
+        <v>10161</v>
       </c>
       <c r="E34" s="7">
         <v>11951</v>
@@ -7109,10 +7109,10 @@
         <v>7068</v>
       </c>
       <c r="C35" s="7">
-        <v>6490</v>
+        <v>7269</v>
       </c>
       <c r="D35" s="7">
-        <v>9329</v>
+        <v>10448</v>
       </c>
       <c r="E35" s="7">
         <v>12208</v>
@@ -7267,10 +7267,10 @@
         <v>7243</v>
       </c>
       <c r="C36" s="7">
-        <v>6651</v>
+        <v>7449</v>
       </c>
       <c r="D36" s="7">
-        <v>9420</v>
+        <v>10550</v>
       </c>
       <c r="E36" s="7">
         <v>12440</v>
@@ -7425,10 +7425,10 @@
         <v>7283</v>
       </c>
       <c r="C37" s="5">
-        <v>6688</v>
+        <v>7491</v>
       </c>
       <c r="D37" s="5">
-        <v>9490</v>
+        <v>10629</v>
       </c>
       <c r="E37" s="5">
         <v>12884</v>
@@ -7583,10 +7583,10 @@
         <v>7338</v>
       </c>
       <c r="C38" s="7">
-        <v>6738</v>
+        <v>7547</v>
       </c>
       <c r="D38" s="7">
-        <v>9677</v>
+        <v>10838</v>
       </c>
       <c r="E38" s="7">
         <v>12908</v>
@@ -7741,10 +7741,10 @@
         <v>7377</v>
       </c>
       <c r="C39" s="7">
-        <v>6774</v>
+        <v>7587</v>
       </c>
       <c r="D39" s="7">
-        <v>9747</v>
+        <v>10917</v>
       </c>
       <c r="E39" s="7">
         <v>13172</v>
@@ -7899,10 +7899,10 @@
         <v>7431</v>
       </c>
       <c r="C40" s="7">
-        <v>6824</v>
+        <v>7643</v>
       </c>
       <c r="D40" s="7">
-        <v>9840</v>
+        <v>11021</v>
       </c>
       <c r="E40" s="7">
         <v>13517</v>
@@ -8057,10 +8057,10 @@
         <v>7487</v>
       </c>
       <c r="C41" s="7">
-        <v>6875</v>
+        <v>7700</v>
       </c>
       <c r="D41" s="7">
-        <v>9966</v>
+        <v>11162</v>
       </c>
       <c r="E41" s="7">
         <v>13622</v>
@@ -8215,10 +8215,10 @@
         <v>7542</v>
       </c>
       <c r="C42" s="7">
-        <v>6926</v>
+        <v>7757</v>
       </c>
       <c r="D42" s="7">
-        <v>10463</v>
+        <v>11719</v>
       </c>
       <c r="E42" s="7">
         <v>13808</v>
@@ -8373,10 +8373,10 @@
         <v>7598</v>
       </c>
       <c r="C43" s="7">
-        <v>6977</v>
+        <v>7814</v>
       </c>
       <c r="D43" s="7">
-        <v>10698</v>
+        <v>11982</v>
       </c>
       <c r="E43" s="7">
         <v>14076</v>
@@ -8531,10 +8531,10 @@
         <v>7939</v>
       </c>
       <c r="C44" s="7">
-        <v>7290</v>
+        <v>8165</v>
       </c>
       <c r="D44" s="7">
-        <v>11184</v>
+        <v>12526</v>
       </c>
       <c r="E44" s="7">
         <v>14424</v>
@@ -8689,10 +8689,10 @@
         <v>8174</v>
       </c>
       <c r="C45" s="7">
-        <v>7506</v>
+        <v>8407</v>
       </c>
       <c r="D45" s="7">
-        <v>11668</v>
+        <v>13068</v>
       </c>
       <c r="E45" s="7">
         <v>15097</v>
@@ -8847,10 +8847,10 @@
         <v>8480</v>
       </c>
       <c r="C46" s="7">
-        <v>7787</v>
+        <v>8721</v>
       </c>
       <c r="D46" s="7">
-        <v>12197</v>
+        <v>13661</v>
       </c>
       <c r="E46" s="7">
         <v>16015</v>
@@ -9005,10 +9005,10 @@
         <v>8805</v>
       </c>
       <c r="C47" s="7">
-        <v>8085</v>
+        <v>9055</v>
       </c>
       <c r="D47" s="7">
-        <v>12728</v>
+        <v>14255</v>
       </c>
       <c r="E47" s="7">
         <v>16816</v>
@@ -9163,10 +9163,10 @@
         <v>9120</v>
       </c>
       <c r="C48" s="7">
-        <v>8375</v>
+        <v>9380</v>
       </c>
       <c r="D48" s="7">
-        <v>13561</v>
+        <v>15188</v>
       </c>
       <c r="E48" s="7">
         <v>17778</v>
@@ -9321,10 +9321,10 @@
         <v>9505</v>
       </c>
       <c r="C49" s="7">
-        <v>8728</v>
+        <v>9775</v>
       </c>
       <c r="D49" s="7">
-        <v>14102</v>
+        <v>15794</v>
       </c>
       <c r="E49" s="7">
         <v>18334</v>
@@ -9479,10 +9479,10 @@
         <v>9755</v>
       </c>
       <c r="C50" s="7">
-        <v>8958</v>
+        <v>10033</v>
       </c>
       <c r="D50" s="7">
-        <v>14642</v>
+        <v>16399</v>
       </c>
       <c r="E50" s="7">
         <v>19053</v>
@@ -9637,10 +9637,10 @@
         <v>9986</v>
       </c>
       <c r="C51" s="7">
-        <v>9170</v>
+        <v>10270</v>
       </c>
       <c r="D51" s="7">
-        <v>15115</v>
+        <v>16929</v>
       </c>
       <c r="E51" s="7">
         <v>19851</v>
@@ -9795,10 +9795,10 @@
         <v>10232</v>
       </c>
       <c r="C52" s="7">
-        <v>9396</v>
+        <v>10524</v>
       </c>
       <c r="D52" s="7">
-        <v>15802</v>
+        <v>17698</v>
       </c>
       <c r="E52" s="7">
         <v>20245</v>
@@ -9953,10 +9953,10 @@
         <v>10479</v>
       </c>
       <c r="C53" s="7">
-        <v>9623</v>
+        <v>10778</v>
       </c>
       <c r="D53" s="7">
-        <v>15967</v>
+        <v>17883</v>
       </c>
       <c r="E53" s="7">
         <v>21005</v>
@@ -10111,10 +10111,10 @@
         <v>10857</v>
       </c>
       <c r="C54" s="7">
-        <v>9970</v>
+        <v>11166</v>
       </c>
       <c r="D54" s="7">
-        <v>17492</v>
+        <v>19591</v>
       </c>
       <c r="E54" s="7">
         <v>22748</v>
@@ -10269,10 +10269,10 @@
         <v>11195</v>
       </c>
       <c r="C55" s="7">
-        <v>10280</v>
+        <v>11514</v>
       </c>
       <c r="D55" s="7">
-        <v>18207</v>
+        <v>20392</v>
       </c>
       <c r="E55" s="7">
         <v>23758</v>
@@ -10427,10 +10427,10 @@
         <v>11528</v>
       </c>
       <c r="C56" s="7">
-        <v>10586</v>
+        <v>11856</v>
       </c>
       <c r="D56" s="7">
-        <v>18923</v>
+        <v>21194</v>
       </c>
       <c r="E56" s="7">
         <v>24754</v>
@@ -10585,10 +10585,10 @@
         <v>12078</v>
       </c>
       <c r="C57" s="7">
-        <v>11091</v>
+        <v>12422</v>
       </c>
       <c r="D57" s="7">
-        <v>20008</v>
+        <v>22409</v>
       </c>
       <c r="E57" s="7">
         <v>25821</v>
@@ -10743,10 +10743,10 @@
         <v>12613</v>
       </c>
       <c r="C58" s="7">
-        <v>11582</v>
+        <v>12972</v>
       </c>
       <c r="D58" s="7">
-        <v>21093</v>
+        <v>23624</v>
       </c>
       <c r="E58" s="7">
         <v>27464</v>
@@ -10901,10 +10901,10 @@
         <v>13349</v>
       </c>
       <c r="C59" s="7">
-        <v>12258</v>
+        <v>13729</v>
       </c>
       <c r="D59" s="7">
-        <v>21194</v>
+        <v>23737</v>
       </c>
       <c r="E59" s="7">
         <v>29052</v>
@@ -11059,10 +11059,10 @@
         <v>13903</v>
       </c>
       <c r="C60" s="7">
-        <v>12767</v>
+        <v>14299</v>
       </c>
       <c r="D60" s="7">
-        <v>22231</v>
+        <v>24899</v>
       </c>
       <c r="E60" s="7">
         <v>30560</v>
@@ -11217,10 +11217,10 @@
         <v>14476</v>
       </c>
       <c r="C61" s="7">
-        <v>13293</v>
+        <v>14888</v>
       </c>
       <c r="D61" s="7">
-        <v>23268</v>
+        <v>26060</v>
       </c>
       <c r="E61" s="7">
         <v>32643</v>
@@ -11375,10 +11375,10 @@
         <v>15345</v>
       </c>
       <c r="C62" s="7">
-        <v>14091</v>
+        <v>15782</v>
       </c>
       <c r="D62" s="7">
-        <v>25855</v>
+        <v>28958</v>
       </c>
       <c r="E62" s="7">
         <v>34291</v>
@@ -11533,10 +11533,10 @@
         <v>16412</v>
       </c>
       <c r="C63" s="7">
-        <v>15071</v>
+        <v>16880</v>
       </c>
       <c r="D63" s="7">
-        <v>27662</v>
+        <v>30981</v>
       </c>
       <c r="E63" s="7">
         <v>35999</v>
@@ -11691,10 +11691,10 @@
         <v>17411</v>
       </c>
       <c r="C64" s="7">
-        <v>15988</v>
+        <v>17907</v>
       </c>
       <c r="D64" s="7">
-        <v>28955</v>
+        <v>32430</v>
       </c>
       <c r="E64" s="7">
         <v>39079</v>
@@ -11849,10 +11849,10 @@
         <v>18498</v>
       </c>
       <c r="C65" s="7">
-        <v>16986</v>
+        <v>19024</v>
       </c>
       <c r="D65" s="7">
-        <v>30660</v>
+        <v>34339</v>
       </c>
       <c r="E65" s="7">
         <v>43151</v>
@@ -12007,10 +12007,10 @@
         <v>19585</v>
       </c>
       <c r="C66" s="7">
-        <v>17984</v>
+        <v>20142</v>
       </c>
       <c r="D66" s="7">
-        <v>32355</v>
+        <v>36238</v>
       </c>
       <c r="E66" s="7">
         <v>48281</v>
@@ -12165,10 +12165,10 @@
         <v>20747</v>
       </c>
       <c r="C67" s="7">
-        <v>19051</v>
+        <v>21337</v>
       </c>
       <c r="D67" s="7">
-        <v>33481</v>
+        <v>37499</v>
       </c>
       <c r="E67" s="7">
         <v>52440</v>
@@ -12323,10 +12323,10 @@
         <v>21963</v>
       </c>
       <c r="C68" s="7">
-        <v>20168</v>
+        <v>22588</v>
       </c>
       <c r="D68" s="7">
-        <v>34880</v>
+        <v>39066</v>
       </c>
       <c r="E68" s="7">
         <v>56687</v>
@@ -12481,10 +12481,10 @@
         <v>23164</v>
       </c>
       <c r="C69" s="7">
-        <v>21271</v>
+        <v>23824</v>
       </c>
       <c r="D69" s="7">
-        <v>36643</v>
+        <v>41040</v>
       </c>
       <c r="E69" s="7">
         <v>58921</v>
@@ -12639,10 +12639,10 @@
         <v>24386</v>
       </c>
       <c r="C70" s="7">
-        <v>22393</v>
+        <v>25080</v>
       </c>
       <c r="D70" s="7">
-        <v>39912</v>
+        <v>44701</v>
       </c>
       <c r="E70" s="7">
         <v>60257</v>
@@ -12797,10 +12797,10 @@
         <v>25599</v>
       </c>
       <c r="C71" s="7">
-        <v>23507</v>
+        <v>26328</v>
       </c>
       <c r="D71" s="7">
-        <v>41788</v>
+        <v>46803</v>
       </c>
       <c r="E71" s="7">
         <v>62245</v>
@@ -12955,10 +12955,10 @@
         <v>26759</v>
       </c>
       <c r="C72" s="5">
-        <v>24572</v>
+        <v>27521</v>
       </c>
       <c r="D72" s="5">
-        <v>43282</v>
+        <v>48476</v>
       </c>
       <c r="E72" s="5">
         <v>63951</v>
@@ -13113,10 +13113,10 @@
         <v>28327</v>
       </c>
       <c r="C73" s="7">
-        <v>26012</v>
+        <v>29133</v>
       </c>
       <c r="D73" s="7">
-        <v>43522</v>
+        <v>48745</v>
       </c>
       <c r="E73" s="7">
         <v>70703</v>
@@ -13271,10 +13271,10 @@
         <v>29332</v>
       </c>
       <c r="C74" s="7">
-        <v>26935</v>
+        <v>30167</v>
       </c>
       <c r="D74" s="7">
-        <v>48393</v>
+        <v>54200</v>
       </c>
       <c r="E74" s="7">
         <v>74620</v>
@@ -13429,10 +13429,10 @@
         <v>30286</v>
       </c>
       <c r="C75" s="7">
-        <v>27811</v>
+        <v>31148</v>
       </c>
       <c r="D75" s="7">
-        <v>49774</v>
+        <v>55747</v>
       </c>
       <c r="E75" s="7">
         <v>78472</v>
@@ -13587,10 +13587,10 @@
         <v>31058</v>
       </c>
       <c r="C76" s="7">
-        <v>28757</v>
+        <v>31920</v>
       </c>
       <c r="D76" s="7">
-        <v>51249</v>
+        <v>56886</v>
       </c>
       <c r="E76" s="7">
         <v>81706</v>
@@ -13745,10 +13745,10 @@
         <v>32413</v>
       </c>
       <c r="C77" s="7">
-        <v>30012</v>
+        <v>33313</v>
       </c>
       <c r="D77" s="7">
-        <v>53223</v>
+        <v>59078</v>
       </c>
       <c r="E77" s="7">
         <v>83193</v>
@@ -13903,10 +13903,10 @@
         <v>33679</v>
       </c>
       <c r="C78" s="7">
-        <v>31184</v>
+        <v>34614</v>
       </c>
       <c r="D78" s="7">
-        <v>55591</v>
+        <v>61706</v>
       </c>
       <c r="E78" s="7">
         <v>88458</v>
@@ -14061,10 +14061,10 @@
         <v>34656</v>
       </c>
       <c r="C79" s="7">
-        <v>32089</v>
+        <v>35619</v>
       </c>
       <c r="D79" s="7">
-        <v>56754</v>
+        <v>62997</v>
       </c>
       <c r="E79" s="7">
         <v>94582</v>
@@ -14219,10 +14219,10 @@
         <v>35932</v>
       </c>
       <c r="C80" s="7">
-        <v>33270</v>
+        <v>36930</v>
       </c>
       <c r="D80" s="7">
-        <v>58589</v>
+        <v>65034</v>
       </c>
       <c r="E80" s="7">
         <v>97235</v>
@@ -14377,10 +14377,10 @@
         <v>37243</v>
       </c>
       <c r="C81" s="7">
-        <v>34484</v>
+        <v>38277</v>
       </c>
       <c r="D81" s="7">
-        <v>60458</v>
+        <v>67108</v>
       </c>
       <c r="E81" s="7">
         <v>100306</v>
@@ -14535,10 +14535,10 @@
         <v>41188</v>
       </c>
       <c r="C82" s="7">
-        <v>38314</v>
+        <v>42337</v>
       </c>
       <c r="D82" s="7">
-        <v>67563</v>
+        <v>74657</v>
       </c>
       <c r="E82" s="7">
         <v>101890</v>
@@ -14693,10 +14693,10 @@
         <v>42532</v>
       </c>
       <c r="C83" s="7">
-        <v>39565</v>
+        <v>43719</v>
       </c>
       <c r="D83" s="7">
-        <v>69794</v>
+        <v>77122</v>
       </c>
       <c r="E83" s="7">
         <v>107790</v>
@@ -14851,10 +14851,10 @@
         <v>43904</v>
       </c>
       <c r="C84" s="7">
-        <v>40841</v>
+        <v>45129</v>
       </c>
       <c r="D84" s="7">
-        <v>71884</v>
+        <v>79432</v>
       </c>
       <c r="E84" s="7">
         <v>110927</v>
@@ -15009,10 +15009,10 @@
         <v>44752</v>
       </c>
       <c r="C85" s="7">
-        <v>41630</v>
+        <v>46001</v>
       </c>
       <c r="D85" s="7">
-        <v>73247</v>
+        <v>80938</v>
       </c>
       <c r="E85" s="7">
         <v>112893</v>
@@ -15167,10 +15167,10 @@
         <v>45999</v>
       </c>
       <c r="C86" s="7">
-        <v>42790</v>
+        <v>47283</v>
       </c>
       <c r="D86" s="7">
-        <v>75335</v>
+        <v>83245</v>
       </c>
       <c r="E86" s="7">
         <v>114681</v>
@@ -15325,10 +15325,10 @@
         <v>47537</v>
       </c>
       <c r="C87" s="7">
-        <v>44220</v>
+        <v>48863</v>
       </c>
       <c r="D87" s="7">
-        <v>77895</v>
+        <v>86074</v>
       </c>
       <c r="E87" s="7">
         <v>116737</v>
@@ -15483,10 +15483,10 @@
         <v>49073</v>
       </c>
       <c r="C88" s="7">
-        <v>45649</v>
+        <v>50442</v>
       </c>
       <c r="D88" s="7">
-        <v>80452</v>
+        <v>88899</v>
       </c>
       <c r="E88" s="7">
         <v>118882</v>
@@ -15641,10 +15641,10 @@
         <v>50755</v>
       </c>
       <c r="C89" s="7">
-        <v>47214</v>
+        <v>52171</v>
       </c>
       <c r="D89" s="7">
-        <v>83001</v>
+        <v>91716</v>
       </c>
       <c r="E89" s="7">
         <v>120759</v>
@@ -15799,10 +15799,10 @@
         <v>51816</v>
       </c>
       <c r="C90" s="7">
-        <v>48201</v>
+        <v>53262</v>
       </c>
       <c r="D90" s="7">
-        <v>84689</v>
+        <v>93581</v>
       </c>
       <c r="E90" s="7">
         <v>122636</v>
@@ -15957,10 +15957,10 @@
         <v>53365</v>
       </c>
       <c r="C91" s="7">
-        <v>49642</v>
+        <v>54854</v>
       </c>
       <c r="D91" s="7">
-        <v>87265</v>
+        <v>96428</v>
       </c>
       <c r="E91" s="7">
         <v>124603</v>
@@ -16115,10 +16115,10 @@
         <v>57132</v>
       </c>
       <c r="C92" s="7">
-        <v>53645</v>
+        <v>58741</v>
       </c>
       <c r="D92" s="7">
-        <v>88716</v>
+        <v>97144</v>
       </c>
       <c r="E92" s="7">
         <v>126570</v>
@@ -16273,10 +16273,10 @@
         <v>59052</v>
       </c>
       <c r="C93" s="7">
-        <v>55448</v>
+        <v>60716</v>
       </c>
       <c r="D93" s="7">
-        <v>90167</v>
+        <v>98733</v>
       </c>
       <c r="E93" s="7">
         <v>128625</v>
@@ -16431,10 +16431,10 @@
         <v>60914</v>
       </c>
       <c r="C94" s="7">
-        <v>57196</v>
+        <v>62630</v>
       </c>
       <c r="D94" s="7">
-        <v>92827</v>
+        <v>101646</v>
       </c>
       <c r="E94" s="7">
         <v>130502</v>
@@ -16589,10 +16589,10 @@
         <v>62239</v>
       </c>
       <c r="C95" s="7">
-        <v>58440</v>
+        <v>63992</v>
       </c>
       <c r="D95" s="7">
-        <v>94791</v>
+        <v>103796</v>
       </c>
       <c r="E95" s="7">
         <v>132468</v>
@@ -16747,10 +16747,10 @@
         <v>64062</v>
       </c>
       <c r="C96" s="7">
-        <v>60152</v>
+        <v>65866</v>
       </c>
       <c r="D96" s="7">
-        <v>97636</v>
+        <v>106911</v>
       </c>
       <c r="E96" s="7">
         <v>134614</v>
@@ -16905,10 +16905,10 @@
         <v>65722</v>
       </c>
       <c r="C97" s="7">
-        <v>61711</v>
+        <v>67574</v>
       </c>
       <c r="D97" s="7">
-        <v>100230</v>
+        <v>109752</v>
       </c>
       <c r="E97" s="7">
         <v>136580</v>
@@ -17063,10 +17063,10 @@
         <v>67446</v>
       </c>
       <c r="C98" s="7">
-        <v>63330</v>
+        <v>69346</v>
       </c>
       <c r="D98" s="7">
-        <v>102917</v>
+        <v>112694</v>
       </c>
       <c r="E98" s="7">
         <v>138636</v>
@@ -17221,10 +17221,10 @@
         <v>69255</v>
       </c>
       <c r="C99" s="7">
-        <v>65028</v>
+        <v>71206</v>
       </c>
       <c r="D99" s="7">
-        <v>105454</v>
+        <v>115472</v>
       </c>
       <c r="E99" s="7">
         <v>141125</v>
@@ -17379,10 +17379,10 @@
         <v>70217</v>
       </c>
       <c r="C100" s="7">
-        <v>65931</v>
+        <v>72194</v>
       </c>
       <c r="D100" s="7">
-        <v>106902</v>
+        <v>117058</v>
       </c>
       <c r="E100" s="7">
         <v>143609</v>
@@ -17537,10 +17537,10 @@
         <v>71825</v>
       </c>
       <c r="C101" s="7">
-        <v>67441</v>
+        <v>73848</v>
       </c>
       <c r="D101" s="7">
-        <v>111317</v>
+        <v>121892</v>
       </c>
       <c r="E101" s="7">
         <v>149539</v>
@@ -17697,8 +17697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B896F2-12D2-429B-9B09-4A097A6AF099}">
   <dimension ref="A1:AZ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM25" sqref="AM25"/>
+    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -17874,10 +17874,10 @@
         <v>5524</v>
       </c>
       <c r="C2" s="5">
-        <v>5211</v>
+        <v>5680</v>
       </c>
       <c r="D2" s="5">
-        <v>7159</v>
+        <v>7803</v>
       </c>
       <c r="E2" s="5">
         <v>8703</v>
@@ -18032,10 +18032,10 @@
         <v>5524</v>
       </c>
       <c r="C3" s="7">
-        <v>5211</v>
+        <v>5680</v>
       </c>
       <c r="D3" s="7">
-        <v>7159</v>
+        <v>7803</v>
       </c>
       <c r="E3" s="7">
         <v>8703</v>
@@ -18190,10 +18190,10 @@
         <v>5524</v>
       </c>
       <c r="C4" s="7">
-        <v>5211</v>
+        <v>5680</v>
       </c>
       <c r="D4" s="7">
-        <v>7159</v>
+        <v>7803</v>
       </c>
       <c r="E4" s="7">
         <v>8703</v>
@@ -18348,10 +18348,10 @@
         <v>5524</v>
       </c>
       <c r="C5" s="7">
-        <v>5211</v>
+        <v>5680</v>
       </c>
       <c r="D5" s="7">
-        <v>7159</v>
+        <v>7803</v>
       </c>
       <c r="E5" s="7">
         <v>8703</v>
@@ -18506,10 +18506,10 @@
         <v>4728</v>
       </c>
       <c r="C6" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D6" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E6" s="7">
         <v>8703</v>
@@ -18664,10 +18664,10 @@
         <v>4728</v>
       </c>
       <c r="C7" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D7" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E7" s="7">
         <v>7956</v>
@@ -18822,10 +18822,10 @@
         <v>4728</v>
       </c>
       <c r="C8" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D8" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E8" s="7">
         <v>7956</v>
@@ -18980,10 +18980,10 @@
         <v>4728</v>
       </c>
       <c r="C9" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D9" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E9" s="7">
         <v>7956</v>
@@ -19138,10 +19138,10 @@
         <v>4728</v>
       </c>
       <c r="C10" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D10" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E10" s="7">
         <v>7956</v>
@@ -19296,10 +19296,10 @@
         <v>4728</v>
       </c>
       <c r="C11" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D11" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E11" s="7">
         <v>7956</v>
@@ -19454,10 +19454,10 @@
         <v>4728</v>
       </c>
       <c r="C12" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D12" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E12" s="7">
         <v>7956</v>
@@ -19612,10 +19612,10 @@
         <v>4728</v>
       </c>
       <c r="C13" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D13" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E13" s="7">
         <v>7956</v>
@@ -19770,10 +19770,10 @@
         <v>4728</v>
       </c>
       <c r="C14" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D14" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E14" s="7">
         <v>7956</v>
@@ -19928,10 +19928,10 @@
         <v>4728</v>
       </c>
       <c r="C15" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D15" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E15" s="7">
         <v>7956</v>
@@ -20086,10 +20086,10 @@
         <v>4728</v>
       </c>
       <c r="C16" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D16" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E16" s="7">
         <v>7956</v>
@@ -20244,10 +20244,10 @@
         <v>4728</v>
       </c>
       <c r="C17" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D17" s="7">
-        <v>6781</v>
+        <v>7595</v>
       </c>
       <c r="E17" s="7">
         <v>7956</v>
@@ -20402,10 +20402,10 @@
         <v>4728</v>
       </c>
       <c r="C18" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D18" s="7">
-        <v>6685</v>
+        <v>7487</v>
       </c>
       <c r="E18" s="7">
         <v>7956</v>
@@ -20560,10 +20560,10 @@
         <v>4728</v>
       </c>
       <c r="C19" s="7">
-        <v>4342</v>
+        <v>4863</v>
       </c>
       <c r="D19" s="7">
-        <v>6802</v>
+        <v>7618</v>
       </c>
       <c r="E19" s="7">
         <v>7956</v>
@@ -20718,10 +20718,10 @@
         <v>4647</v>
       </c>
       <c r="C20" s="7">
-        <v>4267</v>
+        <v>4779</v>
       </c>
       <c r="D20" s="7">
-        <v>6770</v>
+        <v>7582</v>
       </c>
       <c r="E20" s="7">
         <v>8177</v>
@@ -20876,10 +20876,10 @@
         <v>3718</v>
       </c>
       <c r="C21" s="7">
-        <v>3414</v>
+        <v>3824</v>
       </c>
       <c r="D21" s="7">
-        <v>6484</v>
+        <v>7262</v>
       </c>
       <c r="E21" s="7">
         <v>8244</v>
@@ -21034,10 +21034,10 @@
         <v>3754</v>
       </c>
       <c r="C22" s="7">
-        <v>3447</v>
+        <v>3861</v>
       </c>
       <c r="D22" s="7">
-        <v>6398</v>
+        <v>7166</v>
       </c>
       <c r="E22" s="7">
         <v>8437</v>
@@ -21192,10 +21192,10 @@
         <v>3696</v>
       </c>
       <c r="C23" s="7">
-        <v>3394</v>
+        <v>3801</v>
       </c>
       <c r="D23" s="7">
-        <v>6288</v>
+        <v>7043</v>
       </c>
       <c r="E23" s="7">
         <v>8697</v>
@@ -21350,10 +21350,10 @@
         <v>3611</v>
       </c>
       <c r="C24" s="7">
-        <v>3316</v>
+        <v>3714</v>
       </c>
       <c r="D24" s="7">
-        <v>6433</v>
+        <v>7205</v>
       </c>
       <c r="E24" s="7">
         <v>8948</v>
@@ -21508,10 +21508,10 @@
         <v>3644</v>
       </c>
       <c r="C25" s="7">
-        <v>3346</v>
+        <v>3748</v>
       </c>
       <c r="D25" s="7">
-        <v>6579</v>
+        <v>7368</v>
       </c>
       <c r="E25" s="7">
         <v>9131</v>
@@ -21666,10 +21666,10 @@
         <v>3682</v>
       </c>
       <c r="C26" s="7">
-        <v>3381</v>
+        <v>3787</v>
       </c>
       <c r="D26" s="7">
-        <v>6914</v>
+        <v>7744</v>
       </c>
       <c r="E26" s="7">
         <v>9267</v>
@@ -21824,10 +21824,10 @@
         <v>3853</v>
       </c>
       <c r="C27" s="7">
-        <v>3538</v>
+        <v>3963</v>
       </c>
       <c r="D27" s="7">
-        <v>7342</v>
+        <v>8223</v>
       </c>
       <c r="E27" s="7">
         <v>9723</v>
@@ -21982,10 +21982,10 @@
         <v>4082</v>
       </c>
       <c r="C28" s="7">
-        <v>3748</v>
+        <v>4198</v>
       </c>
       <c r="D28" s="7">
-        <v>7773</v>
+        <v>8706</v>
       </c>
       <c r="E28" s="7">
         <v>10254</v>
@@ -22140,10 +22140,10 @@
         <v>4304</v>
       </c>
       <c r="C29" s="7">
-        <v>3952</v>
+        <v>4426</v>
       </c>
       <c r="D29" s="7">
-        <v>7778</v>
+        <v>8711</v>
       </c>
       <c r="E29" s="7">
         <v>10778</v>
@@ -22298,10 +22298,10 @@
         <v>4538</v>
       </c>
       <c r="C30" s="7">
-        <v>4167</v>
+        <v>4667</v>
       </c>
       <c r="D30" s="7">
-        <v>7782</v>
+        <v>8716</v>
       </c>
       <c r="E30" s="7">
         <v>11167</v>
@@ -22456,10 +22456,10 @@
         <v>4751</v>
       </c>
       <c r="C31" s="7">
-        <v>4363</v>
+        <v>4887</v>
       </c>
       <c r="D31" s="7">
-        <v>8165</v>
+        <v>9145</v>
       </c>
       <c r="E31" s="7">
         <v>11417</v>
@@ -22614,10 +22614,10 @@
         <v>4917</v>
       </c>
       <c r="C32" s="7">
-        <v>4515</v>
+        <v>5057</v>
       </c>
       <c r="D32" s="7">
-        <v>8415</v>
+        <v>9425</v>
       </c>
       <c r="E32" s="7">
         <v>11587</v>
@@ -22772,10 +22772,10 @@
         <v>5054</v>
       </c>
       <c r="C33" s="7">
-        <v>4641</v>
+        <v>5198</v>
       </c>
       <c r="D33" s="7">
-        <v>8664</v>
+        <v>9704</v>
       </c>
       <c r="E33" s="7">
         <v>11851</v>
@@ -22930,10 +22930,10 @@
         <v>5210</v>
       </c>
       <c r="C34" s="7">
-        <v>4784</v>
+        <v>5358</v>
       </c>
       <c r="D34" s="7">
-        <v>8782</v>
+        <v>9836</v>
       </c>
       <c r="E34" s="7">
         <v>11951</v>
@@ -23088,10 +23088,10 @@
         <v>5337</v>
       </c>
       <c r="C35" s="7">
-        <v>4901</v>
+        <v>5489</v>
       </c>
       <c r="D35" s="7">
-        <v>9026</v>
+        <v>10109</v>
       </c>
       <c r="E35" s="7">
         <v>12208</v>
@@ -23246,10 +23246,10 @@
         <v>5491</v>
       </c>
       <c r="C36" s="7">
-        <v>5042</v>
+        <v>5647</v>
       </c>
       <c r="D36" s="7">
-        <v>9061</v>
+        <v>10148</v>
       </c>
       <c r="E36" s="7">
         <v>12440</v>
@@ -23404,10 +23404,10 @@
         <v>5568</v>
       </c>
       <c r="C37" s="5">
-        <v>5113</v>
+        <v>5727</v>
       </c>
       <c r="D37" s="5">
-        <v>9149</v>
+        <v>10247</v>
       </c>
       <c r="E37" s="5">
         <v>12884</v>
@@ -23562,10 +23562,10 @@
         <v>5603</v>
       </c>
       <c r="C38" s="7">
-        <v>5145</v>
+        <v>5762</v>
       </c>
       <c r="D38" s="7">
-        <v>9296</v>
+        <v>10412</v>
       </c>
       <c r="E38" s="7">
         <v>12908</v>
@@ -23720,10 +23720,10 @@
         <v>5605</v>
       </c>
       <c r="C39" s="7">
-        <v>5147</v>
+        <v>5765</v>
       </c>
       <c r="D39" s="7">
-        <v>9591</v>
+        <v>10742</v>
       </c>
       <c r="E39" s="7">
         <v>13172</v>
@@ -23878,10 +23878,10 @@
         <v>5607</v>
       </c>
       <c r="C40" s="7">
-        <v>5149</v>
+        <v>5767</v>
       </c>
       <c r="D40" s="7">
-        <v>9591</v>
+        <v>10742</v>
       </c>
       <c r="E40" s="7">
         <v>13517</v>
@@ -24036,10 +24036,10 @@
         <v>5609</v>
       </c>
       <c r="C41" s="7">
-        <v>5151</v>
+        <v>5769</v>
       </c>
       <c r="D41" s="7">
-        <v>9738</v>
+        <v>10907</v>
       </c>
       <c r="E41" s="7">
         <v>13622</v>
@@ -24194,10 +24194,10 @@
         <v>5689</v>
       </c>
       <c r="C42" s="7">
-        <v>5224</v>
+        <v>5851</v>
       </c>
       <c r="D42" s="7">
-        <v>9860</v>
+        <v>11043</v>
       </c>
       <c r="E42" s="7">
         <v>13808</v>
@@ -24352,10 +24352,10 @@
         <v>5920</v>
       </c>
       <c r="C43" s="7">
-        <v>5436</v>
+        <v>6088</v>
       </c>
       <c r="D43" s="7">
-        <v>10431</v>
+        <v>11683</v>
       </c>
       <c r="E43" s="7">
         <v>14076</v>
@@ -24510,10 +24510,10 @@
         <v>6171</v>
       </c>
       <c r="C44" s="7">
-        <v>5667</v>
+        <v>6347</v>
       </c>
       <c r="D44" s="7">
-        <v>11157</v>
+        <v>12496</v>
       </c>
       <c r="E44" s="7">
         <v>14424</v>
@@ -24668,10 +24668,10 @@
         <v>6379</v>
       </c>
       <c r="C45" s="7">
-        <v>5858</v>
+        <v>6561</v>
       </c>
       <c r="D45" s="7">
-        <v>11379</v>
+        <v>12744</v>
       </c>
       <c r="E45" s="7">
         <v>15097</v>
@@ -24826,10 +24826,10 @@
         <v>6667</v>
       </c>
       <c r="C46" s="7">
-        <v>6122</v>
+        <v>6857</v>
       </c>
       <c r="D46" s="7">
-        <v>12254</v>
+        <v>13724</v>
       </c>
       <c r="E46" s="7">
         <v>16015</v>
@@ -24984,10 +24984,10 @@
         <v>6995</v>
       </c>
       <c r="C47" s="7">
-        <v>6423</v>
+        <v>7194</v>
       </c>
       <c r="D47" s="7">
-        <v>12792</v>
+        <v>14327</v>
       </c>
       <c r="E47" s="7">
         <v>16816</v>
@@ -25142,10 +25142,10 @@
         <v>7332</v>
       </c>
       <c r="C48" s="7">
-        <v>6733</v>
+        <v>7541</v>
       </c>
       <c r="D48" s="7">
-        <v>13332</v>
+        <v>14932</v>
       </c>
       <c r="E48" s="7">
         <v>17778</v>
@@ -25300,10 +25300,10 @@
         <v>7846</v>
       </c>
       <c r="C49" s="7">
-        <v>7205</v>
+        <v>8070</v>
       </c>
       <c r="D49" s="7">
-        <v>13972</v>
+        <v>15649</v>
       </c>
       <c r="E49" s="7">
         <v>18334</v>
@@ -25458,10 +25458,10 @@
         <v>8258</v>
       </c>
       <c r="C50" s="7">
-        <v>7583</v>
+        <v>8493</v>
       </c>
       <c r="D50" s="7">
-        <v>14513</v>
+        <v>16255</v>
       </c>
       <c r="E50" s="7">
         <v>19053</v>
@@ -25616,10 +25616,10 @@
         <v>8686</v>
       </c>
       <c r="C51" s="7">
-        <v>7976</v>
+        <v>8933</v>
       </c>
       <c r="D51" s="7">
-        <v>15709</v>
+        <v>17594</v>
       </c>
       <c r="E51" s="7">
         <v>19851</v>
@@ -25774,10 +25774,10 @@
         <v>8802</v>
       </c>
       <c r="C52" s="7">
-        <v>8083</v>
+        <v>9053</v>
       </c>
       <c r="D52" s="7">
-        <v>16204</v>
+        <v>18148</v>
       </c>
       <c r="E52" s="7">
         <v>20245</v>
@@ -25932,10 +25932,10 @@
         <v>8882</v>
       </c>
       <c r="C53" s="7">
-        <v>8156</v>
+        <v>9135</v>
       </c>
       <c r="D53" s="7">
-        <v>16924</v>
+        <v>18955</v>
       </c>
       <c r="E53" s="7">
         <v>21005</v>
@@ -26090,10 +26090,10 @@
         <v>9447</v>
       </c>
       <c r="C54" s="7">
-        <v>8675</v>
+        <v>9716</v>
       </c>
       <c r="D54" s="7">
-        <v>18395</v>
+        <v>20602</v>
       </c>
       <c r="E54" s="7">
         <v>22748</v>
@@ -26248,10 +26248,10 @@
         <v>9922</v>
       </c>
       <c r="C55" s="7">
-        <v>9111</v>
+        <v>10204</v>
       </c>
       <c r="D55" s="7">
-        <v>19149</v>
+        <v>21447</v>
       </c>
       <c r="E55" s="7">
         <v>23758</v>
@@ -26406,10 +26406,10 @@
         <v>10408</v>
       </c>
       <c r="C56" s="7">
-        <v>9557</v>
+        <v>10704</v>
       </c>
       <c r="D56" s="7">
-        <v>20094</v>
+        <v>22505</v>
       </c>
       <c r="E56" s="7">
         <v>24754</v>
@@ -26564,10 +26564,10 @@
         <v>11090</v>
       </c>
       <c r="C57" s="7">
-        <v>10184</v>
+        <v>11406</v>
       </c>
       <c r="D57" s="7">
-        <v>21247</v>
+        <v>23797</v>
       </c>
       <c r="E57" s="7">
         <v>25821</v>
@@ -26722,10 +26722,10 @@
         <v>11793</v>
       </c>
       <c r="C58" s="7">
-        <v>10829</v>
+        <v>12128</v>
       </c>
       <c r="D58" s="7">
-        <v>23580</v>
+        <v>26410</v>
       </c>
       <c r="E58" s="7">
         <v>27464</v>
@@ -26880,10 +26880,10 @@
         <v>12677</v>
       </c>
       <c r="C59" s="7">
-        <v>11641</v>
+        <v>13038</v>
       </c>
       <c r="D59" s="7">
-        <v>25030</v>
+        <v>28034</v>
       </c>
       <c r="E59" s="7">
         <v>29052</v>
@@ -27038,10 +27038,10 @@
         <v>13377</v>
       </c>
       <c r="C60" s="7">
-        <v>12284</v>
+        <v>13758</v>
       </c>
       <c r="D60" s="7">
-        <v>26260</v>
+        <v>29411</v>
       </c>
       <c r="E60" s="7">
         <v>30560</v>
@@ -27196,10 +27196,10 @@
         <v>14062</v>
       </c>
       <c r="C61" s="7">
-        <v>12913</v>
+        <v>14463</v>
       </c>
       <c r="D61" s="7">
-        <v>27485</v>
+        <v>30783</v>
       </c>
       <c r="E61" s="7">
         <v>32643</v>
@@ -27354,10 +27354,10 @@
         <v>15246</v>
       </c>
       <c r="C62" s="7">
-        <v>14000</v>
+        <v>15680</v>
       </c>
       <c r="D62" s="7">
-        <v>28607</v>
+        <v>32040</v>
       </c>
       <c r="E62" s="7">
         <v>34291</v>
@@ -27512,10 +27512,10 @@
         <v>16263</v>
       </c>
       <c r="C63" s="7">
-        <v>14934</v>
+        <v>16726</v>
       </c>
       <c r="D63" s="7">
-        <v>30556</v>
+        <v>34223</v>
       </c>
       <c r="E63" s="7">
         <v>35999</v>
@@ -27670,10 +27670,10 @@
         <v>17547</v>
       </c>
       <c r="C64" s="7">
-        <v>16113</v>
+        <v>18047</v>
       </c>
       <c r="D64" s="7">
-        <v>31712</v>
+        <v>35517</v>
       </c>
       <c r="E64" s="7">
         <v>39079</v>
@@ -27828,10 +27828,10 @@
         <v>18734</v>
       </c>
       <c r="C65" s="7">
-        <v>17203</v>
+        <v>19267</v>
       </c>
       <c r="D65" s="7">
-        <v>33687</v>
+        <v>37729</v>
       </c>
       <c r="E65" s="7">
         <v>43151</v>
@@ -27986,10 +27986,10 @@
         <v>19942</v>
       </c>
       <c r="C66" s="7">
-        <v>18312</v>
+        <v>20509</v>
       </c>
       <c r="D66" s="7">
-        <v>35670</v>
+        <v>39950</v>
       </c>
       <c r="E66" s="7">
         <v>48281</v>
@@ -28144,10 +28144,10 @@
         <v>21449</v>
       </c>
       <c r="C67" s="7">
-        <v>19696</v>
+        <v>22060</v>
       </c>
       <c r="D67" s="7">
-        <v>38096</v>
+        <v>42668</v>
       </c>
       <c r="E67" s="7">
         <v>52440</v>
@@ -28302,10 +28302,10 @@
         <v>22953</v>
       </c>
       <c r="C68" s="7">
-        <v>21077</v>
+        <v>23606</v>
       </c>
       <c r="D68" s="7">
-        <v>41549</v>
+        <v>46535</v>
       </c>
       <c r="E68" s="7">
         <v>56687</v>
@@ -28460,10 +28460,10 @@
         <v>24758</v>
       </c>
       <c r="C69" s="7">
-        <v>22735</v>
+        <v>25463</v>
       </c>
       <c r="D69" s="7">
-        <v>42780</v>
+        <v>47914</v>
       </c>
       <c r="E69" s="7">
         <v>58921</v>
@@ -28618,10 +28618,10 @@
         <v>26322</v>
       </c>
       <c r="C70" s="7">
-        <v>24171</v>
+        <v>27072</v>
       </c>
       <c r="D70" s="7">
-        <v>45200</v>
+        <v>50624</v>
       </c>
       <c r="E70" s="7">
         <v>60257</v>
@@ -28776,10 +28776,10 @@
         <v>27888</v>
       </c>
       <c r="C71" s="7">
-        <v>25609</v>
+        <v>28682</v>
       </c>
       <c r="D71" s="7">
-        <v>48271</v>
+        <v>54064</v>
       </c>
       <c r="E71" s="7">
         <v>62245</v>
@@ -28934,10 +28934,10 @@
         <v>30737</v>
       </c>
       <c r="C72" s="5">
-        <v>28225</v>
+        <v>31612</v>
       </c>
       <c r="D72" s="5">
-        <v>51222</v>
+        <v>57369</v>
       </c>
       <c r="E72" s="5">
         <v>63951</v>
@@ -29092,10 +29092,10 @@
         <v>32747</v>
       </c>
       <c r="C73" s="7">
-        <v>30071</v>
+        <v>33680</v>
       </c>
       <c r="D73" s="7">
-        <v>54638</v>
+        <v>61195</v>
       </c>
       <c r="E73" s="7">
         <v>70703</v>
@@ -29250,10 +29250,10 @@
         <v>34980</v>
       </c>
       <c r="C74" s="7">
-        <v>32121</v>
+        <v>35976</v>
       </c>
       <c r="D74" s="7">
-        <v>56503</v>
+        <v>63283</v>
       </c>
       <c r="E74" s="7">
         <v>74620</v>
@@ -29408,10 +29408,10 @@
         <v>36340</v>
       </c>
       <c r="C75" s="7">
-        <v>33370</v>
+        <v>37374</v>
       </c>
       <c r="D75" s="7">
-        <v>58402</v>
+        <v>65410</v>
       </c>
       <c r="E75" s="7">
         <v>78472</v>
@@ -29566,10 +29566,10 @@
         <v>37297</v>
       </c>
       <c r="C76" s="7">
-        <v>34534</v>
+        <v>38333</v>
       </c>
       <c r="D76" s="7">
-        <v>59790</v>
+        <v>66367</v>
       </c>
       <c r="E76" s="7">
         <v>81706</v>
@@ -29724,10 +29724,10 @@
         <v>38607</v>
       </c>
       <c r="C77" s="7">
-        <v>35747</v>
+        <v>39679</v>
       </c>
       <c r="D77" s="7">
-        <v>61666</v>
+        <v>68449</v>
       </c>
       <c r="E77" s="7">
         <v>83193</v>
@@ -29882,10 +29882,10 @@
         <v>40023</v>
       </c>
       <c r="C78" s="7">
-        <v>37058</v>
+        <v>41134</v>
       </c>
       <c r="D78" s="7">
-        <v>64287</v>
+        <v>71359</v>
       </c>
       <c r="E78" s="7">
         <v>88458</v>
@@ -30040,10 +30040,10 @@
         <v>42216</v>
       </c>
       <c r="C79" s="7">
-        <v>39089</v>
+        <v>43389</v>
       </c>
       <c r="D79" s="7">
-        <v>67706</v>
+        <v>75154</v>
       </c>
       <c r="E79" s="7">
         <v>94582</v>
@@ -30198,10 +30198,10 @@
         <v>43676</v>
       </c>
       <c r="C80" s="7">
-        <v>40441</v>
+        <v>44890</v>
       </c>
       <c r="D80" s="7">
-        <v>69771</v>
+        <v>77446</v>
       </c>
       <c r="E80" s="7">
         <v>97235</v>
@@ -30356,10 +30356,10 @@
         <v>45121</v>
       </c>
       <c r="C81" s="7">
-        <v>41779</v>
+        <v>46375</v>
       </c>
       <c r="D81" s="7">
-        <v>77513</v>
+        <v>86039</v>
       </c>
       <c r="E81" s="7">
         <v>100306</v>
@@ -30514,10 +30514,10 @@
         <v>49893</v>
       </c>
       <c r="C82" s="7">
-        <v>46412</v>
+        <v>51285</v>
       </c>
       <c r="D82" s="7">
-        <v>78389</v>
+        <v>86620</v>
       </c>
       <c r="E82" s="7">
         <v>101890</v>
@@ -30672,10 +30672,10 @@
         <v>51552</v>
       </c>
       <c r="C83" s="7">
-        <v>47955</v>
+        <v>52990</v>
       </c>
       <c r="D83" s="7">
-        <v>84746</v>
+        <v>93644</v>
       </c>
       <c r="E83" s="7">
         <v>107790</v>
@@ -30830,10 +30830,10 @@
         <v>54404</v>
       </c>
       <c r="C84" s="7">
-        <v>50608</v>
+        <v>55922</v>
       </c>
       <c r="D84" s="7">
-        <v>85665</v>
+        <v>94660</v>
       </c>
       <c r="E84" s="7">
         <v>110927</v>
@@ -30988,10 +30988,10 @@
         <v>55970</v>
       </c>
       <c r="C85" s="7">
-        <v>52065</v>
+        <v>57532</v>
       </c>
       <c r="D85" s="7">
-        <v>88191</v>
+        <v>97451</v>
       </c>
       <c r="E85" s="7">
         <v>112893</v>
@@ -31146,10 +31146,10 @@
         <v>57732</v>
       </c>
       <c r="C86" s="7">
-        <v>53704</v>
+        <v>59343</v>
       </c>
       <c r="D86" s="7">
-        <v>90974</v>
+        <v>100526</v>
       </c>
       <c r="E86" s="7">
         <v>114681</v>
@@ -31304,10 +31304,10 @@
         <v>59775</v>
       </c>
       <c r="C87" s="7">
-        <v>55605</v>
+        <v>61444</v>
       </c>
       <c r="D87" s="7">
-        <v>94217</v>
+        <v>104110</v>
       </c>
       <c r="E87" s="7">
         <v>116737</v>
@@ -31462,10 +31462,10 @@
         <v>61779</v>
       </c>
       <c r="C88" s="7">
-        <v>57469</v>
+        <v>63503</v>
       </c>
       <c r="D88" s="7">
-        <v>101759</v>
+        <v>112444</v>
       </c>
       <c r="E88" s="7">
         <v>118882</v>
@@ -31620,10 +31620,10 @@
         <v>65034</v>
       </c>
       <c r="C89" s="7">
-        <v>60497</v>
+        <v>66849</v>
       </c>
       <c r="D89" s="7">
-        <v>104673</v>
+        <v>115664</v>
       </c>
       <c r="E89" s="7">
         <v>120759</v>
@@ -31778,10 +31778,10 @@
         <v>66816</v>
       </c>
       <c r="C90" s="7">
-        <v>62154</v>
+        <v>68680</v>
       </c>
       <c r="D90" s="7">
-        <v>107857</v>
+        <v>119182</v>
       </c>
       <c r="E90" s="7">
         <v>122636</v>
@@ -31936,10 +31936,10 @@
         <v>68804</v>
       </c>
       <c r="C91" s="7">
-        <v>64004</v>
+        <v>70724</v>
       </c>
       <c r="D91" s="7">
-        <v>109905</v>
+        <v>121445</v>
       </c>
       <c r="E91" s="7">
         <v>124603</v>
@@ -32094,10 +32094,10 @@
         <v>73462</v>
       </c>
       <c r="C92" s="7">
-        <v>68978</v>
+        <v>75531</v>
       </c>
       <c r="D92" s="7">
-        <v>111953</v>
+        <v>122589</v>
       </c>
       <c r="E92" s="7">
         <v>126570</v>
@@ -32252,10 +32252,10 @@
         <v>75855</v>
       </c>
       <c r="C93" s="7">
-        <v>71225</v>
+        <v>77991</v>
       </c>
       <c r="D93" s="7">
-        <v>112817</v>
+        <v>123535</v>
       </c>
       <c r="E93" s="7">
         <v>128625</v>
@@ -32410,10 +32410,10 @@
         <v>79958</v>
       </c>
       <c r="C94" s="7">
-        <v>75078</v>
+        <v>82210</v>
       </c>
       <c r="D94" s="7">
-        <v>119144</v>
+        <v>130463</v>
       </c>
       <c r="E94" s="7">
         <v>130502</v>
@@ -32568,10 +32568,10 @@
         <v>82087</v>
       </c>
       <c r="C95" s="7">
-        <v>77077</v>
+        <v>84399</v>
       </c>
       <c r="D95" s="7">
-        <v>119388</v>
+        <v>130730</v>
       </c>
       <c r="E95" s="7">
         <v>132468</v>
@@ -32726,10 +32726,10 @@
         <v>84565</v>
       </c>
       <c r="C96" s="7">
-        <v>79404</v>
+        <v>86947</v>
       </c>
       <c r="D96" s="7">
-        <v>123060</v>
+        <v>134751</v>
       </c>
       <c r="E96" s="7">
         <v>134614</v>
@@ -32884,10 +32884,10 @@
         <v>86691</v>
       </c>
       <c r="C97" s="7">
-        <v>81400</v>
+        <v>89133</v>
       </c>
       <c r="D97" s="7">
-        <v>126249</v>
+        <v>138243</v>
       </c>
       <c r="E97" s="7">
         <v>136580</v>
@@ -33042,10 +33042,10 @@
         <v>88738</v>
       </c>
       <c r="C98" s="7">
-        <v>83322</v>
+        <v>91238</v>
       </c>
       <c r="D98" s="7">
-        <v>127083</v>
+        <v>139156</v>
       </c>
       <c r="E98" s="7">
         <v>138636</v>
@@ -33200,10 +33200,10 @@
         <v>92622</v>
       </c>
       <c r="C99" s="7">
-        <v>86969</v>
+        <v>95231</v>
       </c>
       <c r="D99" s="7">
-        <v>129364</v>
+        <v>141654</v>
       </c>
       <c r="E99" s="7">
         <v>141125</v>
@@ -33358,10 +33358,10 @@
         <v>94459</v>
       </c>
       <c r="C100" s="7">
-        <v>88694</v>
+        <v>97120</v>
       </c>
       <c r="D100" s="7">
-        <v>131641</v>
+        <v>144147</v>
       </c>
       <c r="E100" s="7">
         <v>143609</v>
@@ -33516,10 +33516,10 @@
         <v>96571</v>
       </c>
       <c r="C101" s="7">
-        <v>90677</v>
+        <v>99291</v>
       </c>
       <c r="D101" s="7">
-        <v>137077</v>
+        <v>150099</v>
       </c>
       <c r="E101" s="7">
         <v>149539</v>

</xml_diff>

<commit_message>
Update saving plan with minimum notional amount check and remove cumulative view
</commit_message>
<xml_diff>
--- a/premiumtable.xlsx
+++ b/premiumtable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chakh\OneDrive\桌面\streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B792D51-7063-493B-9C89-108318DCA438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84365C9D-302C-4FFA-A4AE-C6AD5ED62014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2B5941AF-E55B-4360-8715-EE7BF2DCC1DA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
   <si>
     <t>醫家保</t>
   </si>
@@ -1272,6 +1272,14 @@
     <t>Age</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Plan x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plan X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1716,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AB666C-B717-4DAB-B43C-8A2A713B7A3F}">
-  <dimension ref="A1:AZ101"/>
+  <dimension ref="A1:BA101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1729,7 +1737,7 @@
     <col min="53" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -1886,8 +1894,11 @@
       <c r="AZ1" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="BA1" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -2045,7 +2056,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2203,7 +2214,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2361,7 +2372,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -2519,7 +2530,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -2677,7 +2688,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -2835,7 +2846,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -2993,7 +3004,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -3151,7 +3162,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -3309,7 +3320,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -3467,7 +3478,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -3625,7 +3636,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -3783,7 +3794,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -3941,7 +3952,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -4099,7 +4110,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>14</v>
       </c>
@@ -17695,10 +17706,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B896F2-12D2-429B-9B09-4A097A6AF099}">
-  <dimension ref="A1:AZ101"/>
+  <dimension ref="A1:BA101"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D101"/>
+    <sheetView topLeftCell="U40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BA1" sqref="BA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -17708,7 +17719,7 @@
     <col min="53" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -17865,8 +17876,11 @@
       <c r="AZ1" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="BA1" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -18024,7 +18038,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -18182,7 +18196,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -18340,7 +18354,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -18498,7 +18512,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -18656,7 +18670,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -18814,7 +18828,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -18972,7 +18986,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -19130,7 +19144,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -19288,7 +19302,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -19446,7 +19460,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -19604,7 +19618,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>11</v>
       </c>
@@ -19762,7 +19776,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>12</v>
       </c>
@@ -19920,7 +19934,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>13</v>
       </c>
@@ -20078,7 +20092,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>14</v>
       </c>

</xml_diff>